<commit_message>
updated man hinh cho ngoi
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/WindowsFormsApp2/bin/Debug/Data/Data.xlsx
+++ b/WindowsFormsApp2/WindowsFormsApp2/bin/Debug/Data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WindowsFormsApp2\WindowsFormsApp2\bin\Debug\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6BEDF917-19EE-425D-B681-435B2CBB5223}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{613D8CDA-0E52-4E60-AB3A-D567CF369853}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9285096D-E9BE-4E31-B3A9-605255BE9D86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>STT</t>
   </si>
@@ -148,6 +148,48 @@
   </si>
   <si>
     <t>Quản lý giáo dục</t>
+  </si>
+  <si>
+    <t>So ghe</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>C2</t>
   </si>
 </sst>
 </file>
@@ -519,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BD5EE9-9FDF-410A-AF22-839293E087A2}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,10 +574,11 @@
     <col min="3" max="3" width="29.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="16.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,8 +594,11 @@
       <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -568,8 +614,11 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -585,8 +634,11 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -602,8 +654,11 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -619,8 +674,11 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -636,8 +694,11 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -653,8 +714,11 @@
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -670,8 +734,11 @@
       <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -687,8 +754,11 @@
       <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -704,8 +774,11 @@
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -721,8 +794,11 @@
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -738,8 +814,11 @@
       <c r="E12" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -755,8 +834,11 @@
       <c r="E13" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -772,15 +854,18 @@
       <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>

</xml_diff>

<commit_message>
updated mh cho ngoi
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/WindowsFormsApp2/bin/Debug/Data/Data.xlsx
+++ b/WindowsFormsApp2/WindowsFormsApp2/bin/Debug/Data/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WindowsFormsApp2\WindowsFormsApp2\bin\Debug\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PM Diem Danh\WindowsFormsApp2\bin\Debug\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{613D8CDA-0E52-4E60-AB3A-D567CF369853}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EF4A375F-5302-45DF-A321-555C2EE5B1F5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9285096D-E9BE-4E31-B3A9-605255BE9D86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>STT</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>Lê Thị Diễm Thúy</t>
-  </si>
-  <si>
-    <t>CH04151050</t>
   </si>
   <si>
     <t>Quản lý giáo dục</t>
@@ -564,7 +561,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +592,7 @@
         <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -615,7 +612,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -635,7 +632,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -655,7 +652,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -675,7 +672,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -695,7 +692,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -715,7 +712,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -735,7 +732,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -755,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -775,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -795,7 +792,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -815,7 +812,7 @@
         <v>37</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -835,27 +832,27 @@
         <v>37</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>39</v>
+      <c r="B14" s="1">
+        <v>3113410024</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>